<commit_message>
Added all Static Page - Backend
</commit_message>
<xml_diff>
--- a/database/database.xlsx
+++ b/database/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\TatvaSoft\Projects\Helperland\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FD106A-31DD-428D-AC82-181B68B4A34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294D455F-9639-4AC8-8C04-16D131BA3338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{368F47DD-C9D2-49AE-978E-BDD081E7B96D}"/>
   </bookViews>
@@ -334,67 +334,67 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -717,7 +717,7 @@
   <dimension ref="B2:V35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -747,383 +747,388 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="3" spans="2:14" s="2" customFormat="1" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:14" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="6" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="13" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="2:14" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="7"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="14"/>
     </row>
     <row r="9" spans="2:14" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
     </row>
     <row r="10" spans="2:14" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="K10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="L10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="10" t="s">
+      <c r="M10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N10" s="10" t="s">
+      <c r="N10" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
     </row>
     <row r="12" spans="2:14" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
     </row>
     <row r="17" spans="2:22" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
     </row>
     <row r="18" spans="2:22" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="22" t="s">
+      <c r="G18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="2:22" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
     </row>
     <row r="20" spans="2:22" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
     </row>
     <row r="25" spans="2:22" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="F25" s="14" t="s">
+      <c r="C25" s="23"/>
+      <c r="F25" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="G25" s="14"/>
+      <c r="G25" s="23"/>
     </row>
     <row r="26" spans="2:22" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="G26" s="7" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="27" spans="2:22" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
     </row>
     <row r="28" spans="2:22" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
     </row>
     <row r="32" spans="2:22" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="17"/>
-      <c r="M32" s="17"/>
-      <c r="N32" s="17"/>
-      <c r="O32" s="17"/>
-      <c r="P32" s="17"/>
-      <c r="Q32" s="17"/>
-      <c r="R32" s="17"/>
-      <c r="S32" s="17"/>
-      <c r="T32" s="17"/>
-      <c r="U32" s="17"/>
-      <c r="V32" s="17"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="12"/>
+      <c r="S32" s="12"/>
+      <c r="T32" s="12"/>
+      <c r="U32" s="12"/>
+      <c r="V32" s="12"/>
     </row>
     <row r="33" spans="2:22" ht="69.599999999999994" x14ac:dyDescent="0.3">
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="18" t="s">
+      <c r="D33" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="18" t="s">
+      <c r="E33" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F33" s="18" t="s">
+      <c r="F33" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G33" s="18" t="s">
+      <c r="G33" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="H33" s="18" t="s">
+      <c r="H33" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I33" s="18" t="s">
+      <c r="I33" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="J33" s="18" t="s">
+      <c r="J33" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="K33" s="18" t="s">
+      <c r="K33" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="L33" s="18" t="s">
+      <c r="L33" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M33" s="18" t="s">
+      <c r="M33" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N33" s="18" t="s">
+      <c r="N33" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="O33" s="18" t="s">
+      <c r="O33" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="P33" s="18" t="s">
+      <c r="P33" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="Q33" s="18" t="s">
+      <c r="Q33" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="R33" s="18" t="s">
+      <c r="R33" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="S33" s="18" t="s">
+      <c r="S33" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="T33" s="18" t="s">
+      <c r="T33" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="U33" s="18" t="s">
+      <c r="U33" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="V33" s="18" t="s">
+      <c r="V33" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="34" spans="2:22" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="19" t="s">
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="18"/>
-      <c r="O34" s="18"/>
-      <c r="P34" s="18"/>
-      <c r="Q34" s="18"/>
-      <c r="R34" s="18"/>
-      <c r="S34" s="18"/>
-      <c r="T34" s="19" t="s">
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
+      <c r="R34" s="9"/>
+      <c r="S34" s="9"/>
+      <c r="T34" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="U34" s="19" t="s">
+      <c r="U34" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="V34" s="19" t="s">
+      <c r="V34" s="17" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="35" spans="2:22" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="18"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="18"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="18"/>
-      <c r="N35" s="18"/>
-      <c r="O35" s="18"/>
-      <c r="P35" s="18"/>
-      <c r="Q35" s="18"/>
-      <c r="R35" s="18"/>
-      <c r="S35" s="18"/>
-      <c r="T35" s="20"/>
-      <c r="U35" s="20"/>
-      <c r="V35" s="20"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="9"/>
+      <c r="R35" s="9"/>
+      <c r="S35" s="9"/>
+      <c r="T35" s="18"/>
+      <c r="U35" s="18"/>
+      <c r="V35" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B9:N9"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="F25:G25"/>
     <mergeCell ref="B32:V32"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="F11:F12"/>
@@ -1131,11 +1136,6 @@
     <mergeCell ref="U34:U35"/>
     <mergeCell ref="T34:T35"/>
     <mergeCell ref="J34:J35"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B9:N9"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="F25:G25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>